<commit_message>
additional Users changes the summary totals
</commit_message>
<xml_diff>
--- a/Summary/Registered_users_CABLE.xlsx
+++ b/Summary/Registered_users_CABLE.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="652">
   <si>
     <t xml:space="preserve">NCI ID</t>
   </si>
@@ -1438,6 +1438,462 @@
     <t xml:space="preserve">Chang'an University, Xian</t>
   </si>
   <si>
+    <t xml:space="preserve">Total of 153 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas) on 23 Jan 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">129 researchers other than CSIRO employees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76 institutions other than CSIRO (26 Australian and 50 overseas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 countries other than Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52 students (31 in Australian Univ and others from 8 other countries - Argentina, Brazil, China, Germany, Italy, Saudi Arabia, The Netherlands, USA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Researchers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institutions (not including CSIRO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huiyan Li</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qian Zhang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overseas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monash Geo &amp; Env Sci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jason Beringer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qiudan Dai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monash Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranmalee Bandara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stephen Wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murdoch U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brad Evans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UniMelb Earth Sc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Karoly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNSW CCRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sydney U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChunXia Liang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cate Macinnis-Ng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UniMelb Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zelalem Tesemma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derek Eamus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNSW ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faye Cruz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melanie Zeppel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sarah Schroeder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhys Whitley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Francia Avila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flinders U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caecilia Ewenz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNSW CECSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNSW Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ali Ershadi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matthew McCabe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNSW Rivers &amp; Wetlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jin Lee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNSW Water Research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mick Cai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christoph Rudiger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clara Draper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steven Phipps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Universidade Federal de Vicosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evandro Oliveira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monash Weather &amp; Climate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike Rezny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leonardo Neves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sri Srikanthan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gucas.ac.cn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haibo Wang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dongryeol Ryu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sjziam.ac.cn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Lake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IHSOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicolas Boulain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensheng Weng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anuj Furuacharya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queensland CCCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jianting Chu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monash water Sensitive cities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kerry Nice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeff Exbrayat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macquarie U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin De Kauwe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNSW CoECSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stephen Parkes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hongang Yang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jozef Syktus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garry Willgoose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeffrey Walker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert de Ligt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uea.edu.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paulo Teixeira-Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guijun Yang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beijing Normal Uni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yongjiu Dai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caf.ac.cn (Forestry)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jianfeng Liu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAREERI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yanfen Bai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China met Admin, IAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liang Zhang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yaohui Li</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iap.ac.cn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xiaofeng Guo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">igsnrr.ac.cn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qiang Yu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tea.ac.cn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weidong Guo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ujf-grenoble.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Philippe Choler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indonesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bambang Siswanto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Israel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tel Aviv University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yaakov Anker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sally Archibald</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Universidad Complutense de Madrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volker Rath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meteoswiss.ch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maggie Hendry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">King's College London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sue Grimmond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ureading Meteorology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allan Spessa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NASA GSFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sujay Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NASA JPL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshua Fisher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jay Larson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt Fischer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olivier Merlin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Raupach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roger Gifford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Raison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bill Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom Pagano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fangfang Zhao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stuart Matthews</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qinghai Song</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tingting Shi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helen Cleugh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin dix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ian Enting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul Fraser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanessa Haverd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tony Hirst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jack Katzfey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ray Leuning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashok Luhar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richard Matear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John McGregor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keryn Paul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luigi Renzullo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stephen Roxburgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cathy Trudinger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yongqiang Zhang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMIT University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helmholtz Centre for Environmental Research, Leipzig</t>
+  </si>
+  <si>
     <t xml:space="preserve">69 researchers other than CSIRO employees (not counting Jian Zeng) on 13 Apr 2015</t>
   </si>
   <si>
@@ -1520,621 +1976,6 @@
   </si>
   <si>
     <t xml:space="preserve">28 students (17 in Australian Univ and others from 5 other countries - Argentina, China, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 101 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas, Annette Hirsch) on 31 Aug 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52 institutions other than CSIRO (18 Australian and 34 overseas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 students (18 in Australian Univ and others from 5 other countries - Argentina, China, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 105 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas, Annette Hirsch) on 11 Oct 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">91 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54 institutions other than CSIRO (19 Australian and 35 overseas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 countries other than Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32 students (19 in Australian Univ and others from 6 other countries - Argentina, Brazil, China, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 106 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas, Annette Hirsch) on 24 Nov 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">92 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55 institutions other than CSIRO (20 Australian and 35 overseas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 108 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas, Annette Hirsch) on 21 Dec 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">94 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56 institutions other than CSIRO (21 Australian and 35 overseas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33 students (20 in Australian Univ and others from 6 other countries - Argentina, Brazil, China, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 114 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas, Annette Hirsch) on 21 Mar 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60 institutions other than CSIRO (21 Australian and 39 overseas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35 students (21 in Australian Univ and others from 6 other countries - Argentina, Brazil, China, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 119 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas, Annette Hirsch) on 17 May 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">103 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63 institutions other than CSIRO (21 Australian and 42 overseas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36 students (21 in Australian Univ and others from 6 other countries - Argentina, Brazil, China, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 124 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas, Annette Hirsch) on 28 July 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">108 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64 institutions other than CSIRO (21 Australian and 43 overseas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39 students (23 in Australian Univ and others from 6 other countries - Argentina, Brazil, China, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 129 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas, Annette Hirsch) on 7 Sep 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">110 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66 institutions other than CSIRO (23 Australian and 43 overseas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40 students (24 in Australian Univ and others from 6 other countries - Argentina, Brazil, China, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 130 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas, Annette Hirsch) on 22 Nov 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">111 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41 students (25 in Australian Univ and others from 6 other countries - Argentina, Brazil, China, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 132 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas, Annette Hirsch) on 18 Jan 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">113 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42 students (26 in Australian Univ and others from 6 other countries - Argentina, Brazil, China, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 136 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas) on 21 Mar 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">116 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67 institutions other than CSIRO (23 Australian and 44 overseas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44 students (27 in Australian Univ and others from 7 other countries - Argentina, Brazil, China, Germany, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 143 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas) on 8 June 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72 institutions other than CSIRO (25 Australian and 47 overseas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 countries other than Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48 students (29 in Australian Univ and others from 8 other countries - Argentina, Brazil, China, Germany, Italy, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 146 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas) on 17 Aug 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">126 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75 institutions other than CSIRO (26 Australian and 49 overseas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 countries other than Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49 students (29 in Australian Univ and others from 8 other countries - Argentina, Brazil, China, Germany, Italy, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 149 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas) on 30 Oct 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">129 researchers other than CSIRO employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76 institutions other than CSIRO (26 Australian and 50 overseas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51 students (30 in Australian Univ and others from 8 other countries - Argentina, Brazil, China, Germany, Italy, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of 153 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas) on 23 Jan 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52 students (31 in Australian Univ and others from 8 other countries - Argentina, Brazil, China, Germany, Italy, Saudi Arabia, The Netherlands, USA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Researchers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Institutions (not including CSIRO)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMRC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huiyan Li</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qian Zhang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overseas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monash Geo &amp; Env Sci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jason Beringer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qiudan Dai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monash Engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ranmalee Bandara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stephen Wood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Murdoch U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brad Evans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UniMelb Earth Sc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David Karoly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNSW CCRC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sydney U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChunXia Liang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cate Macinnis-Ng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UniMelb Engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zelalem Tesemma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derek Eamus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNSW ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faye Cruz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melanie Zeppel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sarah Schroeder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rhys Whitley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Francia Avila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flinders U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caecilia Ewenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNSW CECSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNSW Engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ali Ershadi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matthew McCabe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNSW Rivers &amp; Wetlands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jin Lee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNSW Water Research</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mick Cai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christoph Rudiger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clara Draper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steven Phipps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Universidade Federal de Vicosa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evandro Oliveira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monash Weather &amp; Climate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike Rezny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leonardo Neves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sri Srikanthan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gucas.ac.cn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haibo Wang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dongryeol Ryu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sjziam.ac.cn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michael Lake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IHSOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicolas Boulain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ensheng Weng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anuj Furuacharya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Queensland CCCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jianting Chu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monash water Sensitive cities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kerry Nice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeff Exbrayat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macquarie U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martin De Kauwe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNSW CoECSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stephen Parkes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hongang Yang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adam Smith</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jozef Syktus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Garry Willgoose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeffrey Walker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robert de Ligt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uea.edu.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paulo Teixeira-Silva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">??</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guijun Yang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beijing Normal Uni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yongjiu Dai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caf.ac.cn (Forestry)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jianfeng Liu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAREERI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yanfen Bai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">China met Admin, IAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liang Zhang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yaohui Li</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iap.ac.cn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xiaofeng Guo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">igsnrr.ac.cn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qiang Yu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tea.ac.cn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weidong Guo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ujf-grenoble.fr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Philippe Choler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indonesia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bambang Siswanto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Israel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tel Aviv University</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yaakov Anker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sally Archibald</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Universidad Complutense de Madrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volker Rath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meteoswiss.ch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maggie Hendry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">King's College London</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sue Grimmond</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ureading Meteorology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allan Spessa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NASA GSFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sujay Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NASA JPL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joshua Fisher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jay Larson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matt Fischer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Olivier Merlin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michael Raupach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roger Gifford</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John Raison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bill Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tom Pagano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fangfang Zhao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stuart Matthews</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qinghai Song</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tingting Shi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Helen Cleugh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martin dix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ian Enting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul Fraser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanessa Haverd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tony Hirst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jack Katzfey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ray Leuning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ashok Luhar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Richard Matear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John McGregor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keryn Paul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luigi Renzullo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stephen Roxburgh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cathy Trudinger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yongqiang Zhang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RMIT University</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Helmholtz Centre for Environmental Research, Leipzig</t>
   </si>
   <si>
     <t xml:space="preserve">Total of 99 researchers (not counting Jian Zeng, Dave Bi and Maciej Golebiewski, and students graduated - Litty Thomas, Annette Hirsch) on 25 July 2016</t>
@@ -2280,20 +2121,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J298"/>
+  <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F88" activeCellId="0" sqref="F88"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A153" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A172" activeCellId="0" sqref="A172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.7767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.093023255814"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.8418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.3767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="18.3348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5427,556 +5268,36 @@
         <v>42838</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C167" s="0" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C168" s="0" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C169" s="0" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C170" s="0" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C171" s="0" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C172" s="0" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C173" s="0" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C174" s="0" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C176" s="0" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C177" s="0" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="0" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C179" s="0" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C181" s="0" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C182" s="0" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C183" s="0" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C184" s="0" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C186" s="0" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C187" s="0" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C188" s="0" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="189" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C189" s="0" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="190" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C190" s="0" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="192" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C192" s="0" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="193" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C193" s="0" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C194" s="0" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="195" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C195" s="0" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C196" s="0" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C198" s="0" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="199" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C199" s="0" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C200" s="0" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="201" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C201" s="0" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="202" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C202" s="0" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="204" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C204" s="0" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="205" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C205" s="0" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="206" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C206" s="0" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="207" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C207" s="0" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="208" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C208" s="0" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="210" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C210" s="0" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C211" s="0" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="212" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C212" s="0" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="213" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C213" s="0" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="214" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C214" s="0" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="216" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C216" s="0" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="217" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C217" s="0" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="218" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C218" s="0" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="219" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C219" s="0" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="220" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C220" s="0" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="222" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C222" s="0" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="223" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C223" s="0" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="224" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C224" s="0" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="225" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C225" s="0" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="226" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C226" s="0" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="228" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C228" s="0" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C229" s="0" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="230" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C230" s="0" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="231" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C231" s="0" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="232" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C232" s="0" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="234" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C234" s="0" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="235" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C235" s="0" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="236" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C236" s="0" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="237" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C237" s="0" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="238" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C238" s="0" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="240" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C240" s="0" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="241" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C241" s="0" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="242" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C242" s="0" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="243" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C243" s="0" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="244" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C244" s="0" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="246" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C246" s="0" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="247" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C247" s="0" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="248" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C248" s="0" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="249" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C249" s="0" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="250" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C250" s="0" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="252" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C252" s="0" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="253" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C253" s="0" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="254" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C254" s="0" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="255" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C255" s="0" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="256" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C256" s="0" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="258" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C258" s="0" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="259" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C259" s="0" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="260" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C260" s="0" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="261" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C261" s="0" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="262" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C262" s="0" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="264" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C264" s="0" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="265" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C265" s="0" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="266" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C266" s="0" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="267" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C267" s="0" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="268" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C268" s="0" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="270" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C270" s="0" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="271" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C271" s="0" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="272" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C272" s="0" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="273" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C273" s="0" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="274" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C274" s="0" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="276" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C276" s="0" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="277" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C277" s="0" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="278" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C278" s="0" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="279" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C279" s="0" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="280" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C280" s="0" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="282" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C282" s="0" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="283" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C283" s="0" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="284" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C284" s="0" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="285" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C285" s="0" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="286" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C286" s="0" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="288" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C288" s="0" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="289" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C289" s="0" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="290" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C290" s="0" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="291" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C291" s="0" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="292" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C292" s="0" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C294" s="0" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C295" s="0" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C296" s="0" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C297" s="0" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C298" s="0" t="s">
-        <v>556</v>
-      </c>
-    </row>
+    <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -6001,19 +5322,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7674418604651"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.4139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>557</v>
+        <v>476</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>558</v>
+        <v>477</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>559</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6021,10 +5342,10 @@
         <v>39295</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>561</v>
+        <v>480</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>179</v>
@@ -6033,16 +5354,16 @@
         <v>40452</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>76</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>562</v>
+        <v>481</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>19</v>
@@ -6053,10 +5374,10 @@
         <v>39295</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>561</v>
+        <v>480</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>279</v>
@@ -6065,16 +5386,16 @@
         <v>40452</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>76</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>563</v>
+        <v>482</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>564</v>
+        <v>483</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>23</v>
@@ -6085,25 +5406,25 @@
         <v>39295</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>565</v>
+        <v>484</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>566</v>
+        <v>485</v>
       </c>
       <c r="G4" s="6" t="n">
         <v>40695</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>76</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>567</v>
+        <v>486</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6111,10 +5432,10 @@
         <v>39295</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>565</v>
+        <v>484</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>364</v>
@@ -6123,13 +5444,13 @@
         <v>40299</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>568</v>
+        <v>487</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>569</v>
+        <v>488</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6137,25 +5458,25 @@
         <v>39417</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>565</v>
+        <v>484</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>570</v>
+        <v>489</v>
       </c>
       <c r="G6" s="6" t="n">
         <v>39934</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>571</v>
+        <v>490</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>572</v>
+        <v>491</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6163,22 +5484,22 @@
         <v>39417</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>573</v>
+        <v>492</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>574</v>
+        <v>493</v>
       </c>
       <c r="G7" s="6" t="n">
         <v>40575</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>571</v>
+        <v>490</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>190</v>
@@ -6189,10 +5510,10 @@
         <v>39417</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>186</v>
@@ -6201,13 +5522,13 @@
         <v>40695</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>576</v>
+        <v>495</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>577</v>
+        <v>496</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6215,25 +5536,25 @@
         <v>39417</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>274</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>578</v>
+        <v>497</v>
       </c>
       <c r="G9" s="6" t="n">
         <v>41091</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>579</v>
+        <v>498</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>580</v>
+        <v>499</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6241,22 +5562,22 @@
         <v>39417</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>274</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>581</v>
+        <v>500</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>582</v>
+        <v>501</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>583</v>
+        <v>502</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6264,25 +5585,25 @@
         <v>39417</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>274</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>584</v>
+        <v>503</v>
       </c>
       <c r="G11" s="6" t="n">
         <v>40238</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>585</v>
+        <v>504</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6290,25 +5611,25 @@
         <v>39417</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>274</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>586</v>
+        <v>505</v>
       </c>
       <c r="G12" s="6" t="n">
         <v>40940</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>587</v>
+        <v>506</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6316,22 +5637,22 @@
         <v>39479</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>588</v>
+        <v>507</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>589</v>
+        <v>508</v>
       </c>
       <c r="G13" s="6" t="n">
         <v>40940</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>590</v>
+        <v>509</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>57</v>
@@ -6342,10 +5663,10 @@
         <v>39508</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>152</v>
@@ -6354,13 +5675,13 @@
         <v>40299</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>591</v>
+        <v>510</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>592</v>
+        <v>511</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6368,22 +5689,22 @@
         <v>39508</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>591</v>
+        <v>510</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>593</v>
+        <v>512</v>
       </c>
       <c r="G15" s="6" t="n">
         <v>41214</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>594</v>
+        <v>513</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>138</v>
@@ -6394,25 +5715,25 @@
         <v>39539</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>561</v>
+        <v>480</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>595</v>
+        <v>514</v>
       </c>
       <c r="G16" s="6" t="n">
         <v>39845</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>596</v>
+        <v>515</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>597</v>
+        <v>516</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6420,19 +5741,19 @@
         <v>39661</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>579</v>
+        <v>498</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>598</v>
+        <v>517</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>599</v>
+        <v>518</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6440,13 +5761,13 @@
         <v>39722</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>600</v>
+        <v>519</v>
       </c>
       <c r="G18" s="6" t="n">
         <v>39600</v>
@@ -6455,10 +5776,10 @@
         <v>222</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>601</v>
+        <v>520</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>602</v>
+        <v>521</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6466,13 +5787,13 @@
         <v>39753</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>603</v>
+        <v>522</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>604</v>
+        <v>523</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>39600</v>
@@ -6481,10 +5802,10 @@
         <v>222</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>601</v>
+        <v>520</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>605</v>
+        <v>524</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6492,13 +5813,13 @@
         <v>39783</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>561</v>
+        <v>480</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>606</v>
+        <v>525</v>
       </c>
       <c r="G20" s="6" t="n">
         <v>40817</v>
@@ -6507,10 +5828,10 @@
         <v>87</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>607</v>
+        <v>526</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>608</v>
+        <v>527</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6518,13 +5839,13 @@
         <v>39845</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>579</v>
+        <v>498</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>609</v>
+        <v>528</v>
       </c>
       <c r="G21" s="6" t="n">
         <v>41091</v>
@@ -6533,7 +5854,7 @@
         <v>87</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>610</v>
+        <v>529</v>
       </c>
       <c r="J21" s="0" t="s">
         <v>452</v>
@@ -6544,13 +5865,13 @@
         <v>40238</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>274</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>611</v>
+        <v>530</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>40634</v>
@@ -6559,7 +5880,7 @@
         <v>464</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>612</v>
+        <v>531</v>
       </c>
       <c r="J22" s="0" t="s">
         <v>462</v>
@@ -6570,13 +5891,13 @@
         <v>40299</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>274</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>613</v>
+        <v>532</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>39753</v>
@@ -6585,10 +5906,10 @@
         <v>45</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>614</v>
+        <v>533</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>615</v>
+        <v>534</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6596,10 +5917,10 @@
         <v>40422</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>573</v>
+        <v>492</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>367</v>
@@ -6611,10 +5932,10 @@
         <v>45</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>614</v>
+        <v>533</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>616</v>
+        <v>535</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6622,7 +5943,7 @@
         <v>40422</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>274</v>
@@ -6637,7 +5958,7 @@
         <v>45</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>614</v>
+        <v>533</v>
       </c>
       <c r="J25" s="0" t="s">
         <v>208</v>
@@ -6648,13 +5969,13 @@
         <v>40664</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>617</v>
+        <v>536</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>618</v>
+        <v>537</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6662,10 +5983,10 @@
         <v>40725</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>579</v>
+        <v>498</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>384</v>
@@ -6676,13 +5997,13 @@
         <v>40756</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>619</v>
+        <v>538</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>620</v>
+        <v>539</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6690,13 +6011,13 @@
         <v>40756</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>621</v>
+        <v>540</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6704,13 +6025,13 @@
         <v>40940</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>622</v>
+        <v>541</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>623</v>
+        <v>542</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6718,10 +6039,10 @@
         <v>41030</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>624</v>
+        <v>543</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>239</v>
@@ -6732,13 +6053,13 @@
         <v>41122</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>625</v>
+        <v>544</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6746,43 +6067,43 @@
         <v>41183</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>626</v>
+        <v>545</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>561</v>
+        <v>480</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>627</v>
+        <v>546</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>617</v>
+        <v>536</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>628</v>
+        <v>547</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>624</v>
+        <v>543</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>47</v>
@@ -6790,26 +6111,26 @@
     </row>
     <row r="37" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>629</v>
+        <v>548</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>630</v>
+        <v>549</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>631</v>
+        <v>550</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6820,10 +6141,10 @@
         <v>222</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>632</v>
+        <v>551</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>633</v>
+        <v>552</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6834,10 +6155,10 @@
         <v>87</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>634</v>
+        <v>553</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>635</v>
+        <v>554</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6848,10 +6169,10 @@
         <v>87</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>636</v>
+        <v>555</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>637</v>
+        <v>556</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6862,10 +6183,10 @@
         <v>87</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>638</v>
+        <v>557</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>639</v>
+        <v>558</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6876,10 +6197,10 @@
         <v>87</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>640</v>
+        <v>559</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>641</v>
+        <v>560</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6890,10 +6211,10 @@
         <v>87</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>642</v>
+        <v>561</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>643</v>
+        <v>562</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6904,10 +6225,10 @@
         <v>87</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>642</v>
+        <v>561</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>644</v>
+        <v>563</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6918,10 +6239,10 @@
         <v>87</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>645</v>
+        <v>564</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>646</v>
+        <v>565</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6932,10 +6253,10 @@
         <v>87</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>647</v>
+        <v>566</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>648</v>
+        <v>567</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6946,10 +6267,10 @@
         <v>87</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>649</v>
+        <v>568</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>650</v>
+        <v>569</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6960,10 +6281,10 @@
         <v>121</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>651</v>
+        <v>570</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>652</v>
+        <v>571</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6971,13 +6292,13 @@
         <v>40269</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>653</v>
+        <v>572</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>654</v>
+        <v>573</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>655</v>
+        <v>574</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6985,13 +6306,13 @@
         <v>39845</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>656</v>
+        <v>575</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>657</v>
+        <v>576</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>658</v>
+        <v>577</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6999,13 +6320,13 @@
         <v>40725</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>659</v>
+        <v>578</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>28</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>660</v>
+        <v>579</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7013,7 +6334,7 @@
         <v>41122</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>659</v>
+        <v>578</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>28</v>
@@ -7027,13 +6348,13 @@
         <v>40940</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>661</v>
+        <v>580</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>662</v>
+        <v>581</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>663</v>
+        <v>582</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7044,7 +6365,7 @@
         <v>379</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>664</v>
+        <v>583</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>377</v>
@@ -7058,10 +6379,10 @@
         <v>55</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>634</v>
+        <v>553</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>665</v>
+        <v>584</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7072,10 +6393,10 @@
         <v>55</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>666</v>
+        <v>585</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>667</v>
+        <v>586</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7086,10 +6407,10 @@
         <v>55</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>668</v>
+        <v>587</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>669</v>
+        <v>588</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7100,10 +6421,10 @@
         <v>45</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>670</v>
+        <v>589</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>671</v>
+        <v>590</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7114,10 +6435,10 @@
         <v>45</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>672</v>
+        <v>591</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>673</v>
+        <v>592</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7128,7 +6449,7 @@
         <v>45</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>614</v>
+        <v>533</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>146</v>
@@ -7136,17 +6457,17 @@
     </row>
     <row r="63" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D63" s="0" t="s">
-        <v>674</v>
+        <v>593</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D64" s="0" t="s">
-        <v>675</v>
+        <v>594</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D65" s="0" t="s">
-        <v>676</v>
+        <v>595</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7154,13 +6475,13 @@
         <v>39264</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>677</v>
+        <v>596</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7168,13 +6489,13 @@
         <v>39326</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>678</v>
+        <v>597</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7182,13 +6503,13 @@
         <v>39326</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>679</v>
+        <v>598</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7196,13 +6517,13 @@
         <v>39479</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>680</v>
+        <v>599</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7210,13 +6531,13 @@
         <v>39814</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>681</v>
+        <v>600</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7224,13 +6545,13 @@
         <v>40087</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>682</v>
+        <v>601</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7238,13 +6559,13 @@
         <v>40118</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C73" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>683</v>
+        <v>602</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7252,13 +6573,13 @@
         <v>40452</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>684</v>
+        <v>603</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7266,18 +6587,18 @@
         <v>40756</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>685</v>
+        <v>604</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C76" s="0" t="s">
         <v>76</v>
@@ -7288,51 +6609,51 @@
     </row>
     <row r="77" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>686</v>
+        <v>605</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>687</v>
+        <v>606</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>688</v>
+        <v>607</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>689</v>
+        <v>608</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>76</v>
@@ -7343,117 +6664,117 @@
     </row>
     <row r="82" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>690</v>
+        <v>609</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C83" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>691</v>
+        <v>610</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>692</v>
+        <v>611</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>693</v>
+        <v>612</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C86" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>694</v>
+        <v>613</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C87" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>695</v>
+        <v>614</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>696</v>
+        <v>615</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>697</v>
+        <v>616</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>698</v>
+        <v>617</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C91" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>699</v>
+        <v>618</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>76</v>
@@ -7464,24 +6785,24 @@
     </row>
     <row r="93" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>700</v>
+        <v>619</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C94" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>701</v>
+        <v>620</v>
       </c>
     </row>
   </sheetData>
@@ -7508,8 +6829,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4883720930233"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9813953488372"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7517,10 +6838,10 @@
         <v>39295</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>561</v>
+        <v>480</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>179</v>
@@ -7532,10 +6853,10 @@
         <v>55</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>668</v>
+        <v>587</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>669</v>
+        <v>588</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7543,10 +6864,10 @@
         <v>39295</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>561</v>
+        <v>480</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>279</v>
@@ -7558,10 +6879,10 @@
         <v>87</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>636</v>
+        <v>555</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>637</v>
+        <v>556</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7569,13 +6890,13 @@
         <v>39295</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>565</v>
+        <v>484</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>566</v>
+        <v>485</v>
       </c>
       <c r="G3" s="6" t="n">
         <v>39600</v>
@@ -7584,10 +6905,10 @@
         <v>222</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>601</v>
+        <v>520</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>602</v>
+        <v>521</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7595,10 +6916,10 @@
         <v>39295</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>565</v>
+        <v>484</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>364</v>
@@ -7610,10 +6931,10 @@
         <v>222</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>601</v>
+        <v>520</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>605</v>
+        <v>524</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7621,13 +6942,13 @@
         <v>39417</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>565</v>
+        <v>484</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>570</v>
+        <v>489</v>
       </c>
       <c r="G5" s="6" t="n">
         <v>39630</v>
@@ -7636,10 +6957,10 @@
         <v>87</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>647</v>
+        <v>566</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>648</v>
+        <v>567</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7647,13 +6968,13 @@
         <v>39417</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>573</v>
+        <v>492</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>574</v>
+        <v>493</v>
       </c>
       <c r="G6" s="6" t="n">
         <v>39630</v>
@@ -7662,7 +6983,7 @@
         <v>379</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>664</v>
+        <v>583</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>377</v>
@@ -7673,10 +6994,10 @@
         <v>39417</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>186</v>
@@ -7688,10 +7009,10 @@
         <v>45</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>614</v>
+        <v>533</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>615</v>
+        <v>534</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7699,13 +7020,13 @@
         <v>39417</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>274</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>578</v>
+        <v>497</v>
       </c>
       <c r="G8" s="6" t="n">
         <v>39814</v>
@@ -7714,10 +7035,10 @@
         <v>87</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>649</v>
+        <v>568</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>650</v>
+        <v>569</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7725,25 +7046,25 @@
         <v>39417</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>274</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>581</v>
+        <v>500</v>
       </c>
       <c r="G9" s="6" t="n">
         <v>39845</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>656</v>
+        <v>575</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>657</v>
+        <v>576</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>658</v>
+        <v>577</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7751,13 +7072,13 @@
         <v>39417</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>274</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>584</v>
+        <v>503</v>
       </c>
       <c r="G10" s="6" t="n">
         <v>40148</v>
@@ -7766,10 +7087,10 @@
         <v>121</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>651</v>
+        <v>570</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>652</v>
+        <v>571</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7777,13 +7098,13 @@
         <v>39417</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>274</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>586</v>
+        <v>505</v>
       </c>
       <c r="G11" s="6" t="n">
         <v>40238</v>
@@ -7792,10 +7113,10 @@
         <v>87</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>638</v>
+        <v>557</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>639</v>
+        <v>558</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7803,25 +7124,25 @@
         <v>39479</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>588</v>
+        <v>507</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>589</v>
+        <v>508</v>
       </c>
       <c r="G12" s="6" t="n">
         <v>40269</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>653</v>
+        <v>572</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>654</v>
+        <v>573</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>655</v>
+        <v>574</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7829,10 +7150,10 @@
         <v>39508</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>152</v>
@@ -7844,10 +7165,10 @@
         <v>222</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>632</v>
+        <v>551</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>633</v>
+        <v>552</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7855,13 +7176,13 @@
         <v>39508</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>591</v>
+        <v>510</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>593</v>
+        <v>512</v>
       </c>
       <c r="G14" s="6" t="n">
         <v>40452</v>
@@ -7870,10 +7191,10 @@
         <v>87</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>640</v>
+        <v>559</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>641</v>
+        <v>560</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7881,13 +7202,13 @@
         <v>39539</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>561</v>
+        <v>480</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>595</v>
+        <v>514</v>
       </c>
       <c r="G15" s="6" t="n">
         <v>40452</v>
@@ -7896,10 +7217,10 @@
         <v>45</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>672</v>
+        <v>591</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>673</v>
+        <v>592</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7907,13 +7228,13 @@
         <v>39661</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>579</v>
+        <v>498</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>598</v>
+        <v>517</v>
       </c>
       <c r="G16" s="6" t="n">
         <v>40634</v>
@@ -7922,7 +7243,7 @@
         <v>464</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>612</v>
+        <v>531</v>
       </c>
       <c r="J16" s="0" t="s">
         <v>462</v>
@@ -7933,25 +7254,25 @@
         <v>39722</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>600</v>
+        <v>519</v>
       </c>
       <c r="G17" s="6" t="n">
         <v>40725</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>659</v>
+        <v>578</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>28</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>660</v>
+        <v>579</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7959,13 +7280,13 @@
         <v>39753</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>603</v>
+        <v>522</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>604</v>
+        <v>523</v>
       </c>
       <c r="G18" s="6" t="n">
         <v>40787</v>
@@ -7974,10 +7295,10 @@
         <v>87</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>634</v>
+        <v>553</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>635</v>
+        <v>554</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7985,13 +7306,13 @@
         <v>39783</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>561</v>
+        <v>480</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>606</v>
+        <v>525</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>40817</v>
@@ -8000,10 +7321,10 @@
         <v>87</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>607</v>
+        <v>526</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>608</v>
+        <v>527</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8011,13 +7332,13 @@
         <v>39845</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>579</v>
+        <v>498</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>609</v>
+        <v>528</v>
       </c>
       <c r="G20" s="6" t="n">
         <v>40940</v>
@@ -8026,10 +7347,10 @@
         <v>55</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>634</v>
+        <v>553</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>665</v>
+        <v>584</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8037,13 +7358,13 @@
         <v>39845</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>596</v>
+        <v>515</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>597</v>
+        <v>516</v>
       </c>
       <c r="G21" s="6" t="n">
         <v>40940</v>
@@ -8052,10 +7373,10 @@
         <v>55</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>666</v>
+        <v>585</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>667</v>
+        <v>586</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8063,13 +7384,13 @@
         <v>39934</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>571</v>
+        <v>490</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>572</v>
+        <v>491</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>40940</v>
@@ -8078,10 +7399,10 @@
         <v>45</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>614</v>
+        <v>533</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>616</v>
+        <v>535</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8089,25 +7410,25 @@
         <v>40238</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>585</v>
+        <v>504</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>40940</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>661</v>
+        <v>580</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>662</v>
+        <v>581</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>663</v>
+        <v>582</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8115,13 +7436,13 @@
         <v>40238</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>274</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>611</v>
+        <v>530</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>40969</v>
@@ -8130,10 +7451,10 @@
         <v>87</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>645</v>
+        <v>564</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>646</v>
+        <v>565</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8141,13 +7462,13 @@
         <v>40299</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>568</v>
+        <v>487</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>569</v>
+        <v>488</v>
       </c>
       <c r="G25" s="6" t="n">
         <v>41091</v>
@@ -8156,7 +7477,7 @@
         <v>87</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>610</v>
+        <v>529</v>
       </c>
       <c r="J25" s="0" t="s">
         <v>452</v>
@@ -8167,19 +7488,19 @@
         <v>40299</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>591</v>
+        <v>510</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>592</v>
+        <v>511</v>
       </c>
       <c r="G26" s="6" t="n">
         <v>41122</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>659</v>
+        <v>578</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>28</v>
@@ -8193,13 +7514,13 @@
         <v>40299</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>274</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>613</v>
+        <v>532</v>
       </c>
       <c r="G27" s="6" t="n">
         <v>41122</v>
@@ -8208,10 +7529,10 @@
         <v>45</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>670</v>
+        <v>589</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>671</v>
+        <v>590</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8219,10 +7540,10 @@
         <v>40422</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>573</v>
+        <v>492</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>367</v>
@@ -8234,7 +7555,7 @@
         <v>45</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>614</v>
+        <v>533</v>
       </c>
       <c r="J28" s="0" t="s">
         <v>208</v>
@@ -8245,7 +7566,7 @@
         <v>40422</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>274</v>
@@ -8260,10 +7581,10 @@
         <v>87</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>642</v>
+        <v>561</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>643</v>
+        <v>562</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8271,13 +7592,13 @@
         <v>40452</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>562</v>
+        <v>481</v>
       </c>
       <c r="G30" s="6" t="n">
         <v>41244</v>
@@ -8286,10 +7607,10 @@
         <v>87</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>642</v>
+        <v>561</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>644</v>
+        <v>563</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8297,13 +7618,13 @@
         <v>40452</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>563</v>
+        <v>482</v>
       </c>
       <c r="G31" s="6" t="n">
         <v>41244</v>
@@ -8312,7 +7633,7 @@
         <v>45</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>614</v>
+        <v>533</v>
       </c>
       <c r="J31" s="0" t="s">
         <v>146</v>
@@ -8323,10 +7644,10 @@
         <v>40575</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>571</v>
+        <v>490</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>190</v>
@@ -8337,13 +7658,13 @@
         <v>40664</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>617</v>
+        <v>536</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>618</v>
+        <v>537</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8351,13 +7672,13 @@
         <v>40695</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>567</v>
+        <v>486</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8365,13 +7686,13 @@
         <v>40695</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>576</v>
+        <v>495</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>577</v>
+        <v>496</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8379,10 +7700,10 @@
         <v>40725</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>579</v>
+        <v>498</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>384</v>
@@ -8393,13 +7714,13 @@
         <v>40756</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>619</v>
+        <v>538</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>620</v>
+        <v>539</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8407,13 +7728,13 @@
         <v>40756</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>621</v>
+        <v>540</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8421,13 +7742,13 @@
         <v>40940</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>622</v>
+        <v>541</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>623</v>
+        <v>542</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8435,13 +7756,13 @@
         <v>40940</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>587</v>
+        <v>506</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8449,10 +7770,10 @@
         <v>40940</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>590</v>
+        <v>509</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>57</v>
@@ -8463,10 +7784,10 @@
         <v>41030</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>624</v>
+        <v>543</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>239</v>
@@ -8477,13 +7798,13 @@
         <v>41091</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>579</v>
+        <v>498</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>580</v>
+        <v>499</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8491,13 +7812,13 @@
         <v>41122</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>20</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>625</v>
+        <v>544</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8505,13 +7826,13 @@
         <v>41183</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>575</v>
+        <v>494</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>626</v>
+        <v>545</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8519,10 +7840,10 @@
         <v>41214</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>594</v>
+        <v>513</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>138</v>
@@ -8530,43 +7851,43 @@
     </row>
     <row r="47" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>561</v>
+        <v>480</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>627</v>
+        <v>546</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>617</v>
+        <v>536</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>628</v>
+        <v>547</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>582</v>
+        <v>501</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>583</v>
+        <v>502</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>624</v>
+        <v>543</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>47</v>
@@ -8574,34 +7895,34 @@
     </row>
     <row r="51" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>629</v>
+        <v>548</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>630</v>
+        <v>549</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>631</v>
+        <v>550</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>560</v>
+        <v>479</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>599</v>
+        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -8628,11 +7949,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.7767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="17.8418604651163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.3767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="18.3348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9238,7 +8559,7 @@
         <v>448</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>702</v>
+        <v>621</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>10</v>
@@ -9685,7 +9006,7 @@
         <v>309</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>703</v>
+        <v>622</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>226</v>
@@ -10127,202 +9448,202 @@
     </row>
     <row r="99" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="s">
-        <v>471</v>
+        <v>623</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
-        <v>472</v>
+        <v>624</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>473</v>
+        <v>625</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
-        <v>474</v>
+        <v>626</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
-        <v>475</v>
+        <v>627</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="s">
-        <v>476</v>
+        <v>628</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="0" t="s">
-        <v>473</v>
+        <v>625</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
-        <v>477</v>
+        <v>629</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
-        <v>478</v>
+        <v>630</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
-        <v>479</v>
+        <v>631</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="s">
-        <v>473</v>
+        <v>625</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>480</v>
+        <v>632</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>481</v>
+        <v>633</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
-        <v>482</v>
+        <v>634</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="0" t="s">
-        <v>483</v>
+        <v>635</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="0" t="s">
-        <v>484</v>
+        <v>636</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="0" t="s">
-        <v>485</v>
+        <v>637</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="0" t="s">
-        <v>486</v>
+        <v>638</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="0" t="s">
-        <v>487</v>
+        <v>639</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="0" t="s">
-        <v>488</v>
+        <v>640</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="0" t="s">
-        <v>489</v>
+        <v>641</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="0" t="s">
-        <v>490</v>
+        <v>642</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="0" t="s">
-        <v>491</v>
+        <v>643</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="0" t="s">
-        <v>487</v>
+        <v>639</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="0" t="s">
-        <v>488</v>
+        <v>640</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="0" t="s">
-        <v>492</v>
+        <v>644</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="0" t="s">
-        <v>493</v>
+        <v>645</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="0" t="s">
-        <v>491</v>
+        <v>643</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>487</v>
+        <v>639</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="0" t="s">
-        <v>494</v>
+        <v>646</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="0" t="s">
-        <v>495</v>
+        <v>647</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="0" t="s">
-        <v>496</v>
+        <v>648</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="0" t="s">
-        <v>497</v>
+        <v>649</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="0" t="s">
-        <v>487</v>
+        <v>639</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="0" t="s">
-        <v>498</v>
+        <v>650</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="0" t="s">
-        <v>704</v>
+        <v>651</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="0" t="s">
-        <v>485</v>
+        <v>637</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="0" t="s">
-        <v>497</v>
+        <v>649</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="0" t="s">
-        <v>487</v>
+        <v>639</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="0" t="s">
-        <v>498</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>